<commit_message>
update to xbee module catalog
</commit_message>
<xml_diff>
--- a/Xbee module catalog.xlsx
+++ b/Xbee module catalog.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26915"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaypoddar/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaypoddar/Documents/codes/GitHub/parkmesh/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,6 +16,9 @@
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -24,14 +27,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Node Identifier</t>
   </si>
   <si>
-    <t>DM-1</t>
-  </si>
-  <si>
     <t>DM-2</t>
   </si>
   <si>
@@ -50,16 +50,25 @@
     <t>40F96376</t>
   </si>
   <si>
-    <t>DMPCB-1</t>
-  </si>
-  <si>
     <t>40A164C9</t>
   </si>
   <si>
-    <t>DMPCB-2</t>
-  </si>
-  <si>
     <t>40A863C2</t>
+  </si>
+  <si>
+    <t>DMPCB-3</t>
+  </si>
+  <si>
+    <t>DMPCB-4</t>
+  </si>
+  <si>
+    <t>DM-5</t>
+  </si>
+  <si>
+    <t>40F96362</t>
+  </si>
+  <si>
+    <t>DM-6</t>
   </si>
 </sst>
 </file>
@@ -383,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -399,10 +408,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -410,43 +419,54 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
-        <v>11</v>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed the data size issue
The data packet length read should be not fixed to 2 should read all
values. Upload to test
</commit_message>
<xml_diff>
--- a/Xbee module catalog.xlsx
+++ b/Xbee module catalog.xlsx
@@ -47,9 +47,6 @@
     <t>SL</t>
   </si>
   <si>
-    <t>40F96376</t>
-  </si>
-  <si>
     <t>40A164C9</t>
   </si>
   <si>
@@ -68,7 +65,10 @@
     <t>40F96362</t>
   </si>
   <si>
-    <t>DM-6</t>
+    <t>DMWIRE-6</t>
+  </si>
+  <si>
+    <t>40DC1FEF</t>
   </si>
 </sst>
 </file>
@@ -395,7 +395,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -422,34 +422,34 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -460,13 +460,13 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Conflicts resolved from last merge
Conflicts resolved for burak to add his code
</commit_message>
<xml_diff>
--- a/Xbee module catalog.xlsx
+++ b/Xbee module catalog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="780" yWindow="460" windowWidth="14300" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,28 +47,28 @@
     <t>SL</t>
   </si>
   <si>
-    <t>40A164C9</t>
-  </si>
-  <si>
-    <t>40A863C2</t>
-  </si>
-  <si>
-    <t>DMPCB-3</t>
-  </si>
-  <si>
-    <t>DMPCB-4</t>
-  </si>
-  <si>
     <t>DM-5</t>
   </si>
   <si>
     <t>40F96362</t>
   </si>
   <si>
-    <t>DMWIRE-6</t>
-  </si>
-  <si>
-    <t>40DC1FEF</t>
+    <t>DM-1</t>
+  </si>
+  <si>
+    <t>DM-3</t>
+  </si>
+  <si>
+    <t>40F963B6</t>
+  </si>
+  <si>
+    <t>40F96364</t>
+  </si>
+  <si>
+    <t>DM-4</t>
+  </si>
+  <si>
+    <t>40F96376</t>
   </si>
 </sst>
 </file>
@@ -395,7 +395,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -416,7 +416,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -427,7 +427,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -444,12 +444,12 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -470,6 +470,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:C6">
+    <sortCondition ref="A2"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>